<commit_message>
:lipstick: feat: Adição de novos arquivos
</commit_message>
<xml_diff>
--- a/escolas/imaculada conceicao/8C.xlsx
+++ b/escolas/imaculada conceicao/8C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\ACTTEENS\Automatização\escolas\imaculada conceicao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\actteensprogram-automacao\escolas\imaculada conceicao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C5DC8A-8D16-4AC2-94B9-217687D7C0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D6335C-5908-475E-B6DE-D5F0479A1220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1935" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Gian Pedro Duarte da Silva</t>
   </si>
@@ -98,13 +98,55 @@
   </si>
   <si>
     <t>Aluno</t>
+  </si>
+  <si>
+    <t>Alice Ferreira Chagas</t>
+  </si>
+  <si>
+    <t>Amanda Torres Costa</t>
+  </si>
+  <si>
+    <t>Ana Julia Lobo Cardoso</t>
+  </si>
+  <si>
+    <t>Anna Karolina H. Mazza</t>
+  </si>
+  <si>
+    <t>Arthur José de Oliveira Barban</t>
+  </si>
+  <si>
+    <t>Bianca Zabott Potzik</t>
+  </si>
+  <si>
+    <t>Bruna Maria Bueno Rodrigues</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo da Cruz</t>
+  </si>
+  <si>
+    <t>Christoffer Willam Pio Soares</t>
+  </si>
+  <si>
+    <t>Clara Borges Benedito</t>
+  </si>
+  <si>
+    <t>Davi Emanoel Carvalho da Silva</t>
+  </si>
+  <si>
+    <t>Davi Henrique Valença Torres</t>
+  </si>
+  <si>
+    <t>Fellipe de Souza Fagá Garcia</t>
+  </si>
+  <si>
+    <t>Gabriely Vitória de Sousa Martins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +168,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,12 +186,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,12 +245,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -216,14 +256,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,7 +588,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,260 +599,384 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8">
+        <v>5543984779747</v>
+      </c>
+      <c r="C2" s="8">
+        <v>5543984460390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5543996271963</v>
+      </c>
+      <c r="C3" s="8">
+        <v>5543996762736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="8">
+        <v>5543991474430</v>
+      </c>
+      <c r="C4" s="8">
+        <v>5543991109503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8">
+        <v>5543984426167</v>
+      </c>
+      <c r="C5" s="8">
+        <v>5543984421507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8">
+        <v>5543991802918</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5543998055348</v>
+      </c>
+      <c r="C7" s="8">
+        <v>5543999302101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8">
+        <v>5543999299286</v>
+      </c>
+      <c r="C8" s="8">
+        <v>5543999358189</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5543998723883</v>
+      </c>
+      <c r="C9" s="8">
+        <v>5543991189169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8">
+        <v>5543996270937</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="8">
+        <v>5543991685021</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8">
+        <v>5543984837459</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5543991586914</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8">
+        <v>5543991397509</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B16" s="8">
         <v>5543984992522</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C16" s="8">
         <v>5543991825230</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B17" s="8">
         <v>5543991856554</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C17" s="8">
         <v>5543991581876</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B18" s="8">
         <v>5543996256766</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C18" s="8">
         <v>5543996942136</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B19" s="8">
         <v>5543991970904</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C19" s="8">
         <v>5543991216042</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="5">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8">
         <v>5543988178657</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B22" s="8">
         <v>5543996532686</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B23" s="8">
         <v>5543998417021</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C23" s="8">
         <v>5543996212108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B25" s="8">
         <v>5543984596548</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C25" s="8">
         <v>5543984530252</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="5">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8">
         <v>5543999184610</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B27" s="8">
         <v>5543988552451</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C27" s="8">
         <v>5543998148878</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B28" s="8">
         <v>5543996597339</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C28" s="8">
         <v>5543988483413</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B29" s="8">
         <v>5543999753656</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C29" s="8">
         <v>5543996540489</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B30" s="8">
         <v>5543991484298</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C30" s="8">
         <v>5543991862221</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B31" s="8">
         <v>5543999694493</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C31" s="8">
         <v>5543991695157</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="5">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8">
         <v>5543988052775</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8">
-        <v>5543998307941</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B35" s="8">
+        <v>5543998387941</v>
+      </c>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B37" s="8">
         <v>5543999320612</v>
       </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B38" s="8">
         <v>5543991869497</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C38" s="8">
         <v>5543991563482</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>